<commit_message>
working code for all login scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheet/OrangeHRMLogin.xlsx
+++ b/src/test/resources/ExcelSheet/OrangeHRMLogin.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\TestNG_OrangeHRM\src\test\resources\ExcelSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\eclipse-workspace\TestNGFramework_OrangeHRMWebsite\src\test\resources\ExcelSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887B088A-769A-4CDE-B1E4-65826ED45709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDF0265-E1A5-472F-85DE-4C2FEFB895BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{70022871-2514-4B38-B863-26463BC342D3}"/>
   </bookViews>
   <sheets>
     <sheet name="OrangeLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Username</t>
   </si>
@@ -40,29 +39,41 @@
     <t>admin123</t>
   </si>
   <si>
-    <t>dsczdfzs</t>
-  </si>
-  <si>
-    <t>mmnnn657</t>
-  </si>
-  <si>
-    <t>Message</t>
-  </si>
-  <si>
-    <t>DashBoard</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
     <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>ExpectedError</t>
+  </si>
+  <si>
+    <t>ErrorType</t>
+  </si>
+  <si>
+    <t>empty-pass</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>popup</t>
+  </si>
+  <si>
+    <t>empty-user</t>
+  </si>
+  <si>
+    <t>empty-both</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,64 +82,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC5D3FF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -136,32 +106,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D813E5B-CEE3-4DA2-B78D-CA6C5FB8BC57}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,92 +438,80 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="18.44140625" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883776BF-F70D-4428-8F27-187DB5060FB0}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20:H21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>